<commit_message>
Oppdatert for 2. Iterasjon
</commit_message>
<xml_diff>
--- a/Dokumentasjon og MSF/Risikovurdering.xlsx
+++ b/Dokumentasjon og MSF/Risikovurdering.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\Documents\Westerdals\Iterativt Webprosjekt - PJ 2100\Eksamen2100 PJ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\Documents\Westerdals\Iterativt Webprosjekt - PJ 2100\Eksamen2100 PJ\Dokumentasjon og MSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -103,12 +103,160 @@
         </r>
       </text>
     </comment>
+    <comment ref="B19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>eb:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Meget kritisk for prosjektet=10
+Uvesentlig=1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>eb:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Helt sikkert at det inntreffer=1
+Helt usannsynlig=0</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>eb:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Risiko med høyest risikopoeng skal prioriteres først. Benytt sorteringsfunkjonen i excel til å rangere de ulike risiki.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B34" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>eb:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Meget kritisk for prosjektet=10
+Uvesentlig=1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C34" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>eb:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Helt sikkert at det inntreffer=1
+Helt usannsynlig=0</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D34" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>eb:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Risiko med høyest risikopoeng skal prioriteres først. Benytt sorteringsfunkjonen i excel til å rangere de ulike risiki.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="47">
   <si>
     <t>Konsekvens (K)</t>
   </si>
@@ -231,13 +379,31 @@
   </si>
   <si>
     <t>Spre arbeidsoppgavene, øke arbeidstimer for tapt arbeidskraft.</t>
+  </si>
+  <si>
+    <t>V1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prøve å gjennskap tapt data, </t>
+  </si>
+  <si>
+    <t>V1.1 (Revidert)</t>
+  </si>
+  <si>
+    <t>V1.2 (2. iterasjon)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sett realistiske mål basert å gruppens kunskap. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Det primære som har blitt endret fra iterasjon til iterasjon er konsekvensfaktoren, sannsynlighetsprosenten og risikoen det medgjører. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,8 +460,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -306,6 +479,11 @@
       <patternFill patternType="solid">
         <fgColor indexed="13"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -333,11 +511,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -359,8 +538,13 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -640,10 +824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -665,6 +849,11 @@
         <v>30</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
@@ -916,21 +1105,522 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="6">
+        <v>7</v>
+      </c>
+      <c r="C20" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="D20" s="6">
+        <f t="shared" ref="D20:D29" si="1">B20*C20</f>
+        <v>4.2</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="6">
+        <v>9</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D21" s="6">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="6">
+        <v>7</v>
+      </c>
+      <c r="C22" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="D22" s="6">
+        <f t="shared" si="1"/>
+        <v>4.2</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="6">
+        <v>10</v>
+      </c>
+      <c r="C23" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D23" s="6">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="6">
+        <v>4</v>
+      </c>
+      <c r="C24" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="D24" s="6">
+        <f t="shared" si="1"/>
+        <v>1.6</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="6">
+        <v>8.5</v>
+      </c>
+      <c r="C25" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="D25" s="6">
+        <f t="shared" si="1"/>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="8">
+        <v>8</v>
+      </c>
+      <c r="C26" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="D26" s="6">
+        <f t="shared" si="1"/>
+        <v>3.2</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="6">
+        <v>3</v>
+      </c>
+      <c r="C27" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="D27" s="6">
+        <f t="shared" si="1"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="6">
+        <v>5</v>
+      </c>
+      <c r="C28" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="D28" s="6">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="6">
+        <v>6</v>
+      </c>
+      <c r="C29" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="D29" s="6">
+        <f t="shared" si="1"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="12">
+        <v>7.5</v>
+      </c>
+      <c r="C30" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="D30" s="11">
+        <f>B30*C30</f>
+        <v>1.5</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="6">
+        <v>8</v>
+      </c>
+      <c r="C35" s="6">
+        <v>0.35</v>
+      </c>
+      <c r="D35" s="6">
+        <f>B35*C35</f>
+        <v>2.8</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="6">
+        <v>6</v>
+      </c>
+      <c r="C36" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="D36" s="6">
+        <f t="shared" ref="D35:D44" si="2">B36*C36</f>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="6">
+        <v>7</v>
+      </c>
+      <c r="C37" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D37" s="6">
+        <f t="shared" si="2"/>
+        <v>3.5</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="6">
+        <v>10</v>
+      </c>
+      <c r="C38" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="D38" s="6">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" s="6">
+        <v>4</v>
+      </c>
+      <c r="C39" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="D39" s="6">
+        <f t="shared" si="2"/>
+        <v>1.6</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" s="6">
+        <v>8.5</v>
+      </c>
+      <c r="C40" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="D40" s="6">
+        <f t="shared" si="2"/>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="8">
+        <v>8</v>
+      </c>
+      <c r="C41" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="D41" s="6">
+        <f t="shared" si="2"/>
+        <v>3.2</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" s="6">
+        <v>3</v>
+      </c>
+      <c r="C42" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="D42" s="6">
+        <f t="shared" si="2"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="6">
+        <v>5</v>
+      </c>
+      <c r="C43" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="D43" s="6">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B44" s="6">
+        <v>6</v>
+      </c>
+      <c r="C44" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="D44" s="6">
+        <f t="shared" si="2"/>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" s="12">
+        <v>9</v>
+      </c>
+      <c r="C45" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="D45" s="11">
+        <f>B45*C45</f>
+        <v>1.8</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A48" s="14" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>